<commit_message>
add Scoreboard BUG when restarting
</commit_message>
<xml_diff>
--- a/WorkLogFlorian.xlsx
+++ b/WorkLogFlorian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH\GitRepo\FH_BIF5_CGRMR_OpenGL-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340F8262-8BEC-40DF-9675-4C3AE813B92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C7A1EE-34DB-44DE-AC13-7D464D5C6943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Flo</t>
   </si>
@@ -36,13 +36,22 @@
     <t>Project setup</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Time(h)</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Score on Window</t>
+  </si>
+  <si>
+    <t>Direction Light</t>
   </si>
 </sst>
 </file>
@@ -78,10 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -362,17 +372,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L3"/>
+  <dimension ref="B1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
@@ -389,24 +400,70 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
         <v>45677</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.875</v>
       </c>
       <c r="H3" s="2"/>
       <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>3.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45678</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45679</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>